<commit_message>
Metricas de proeycto v2
</commit_message>
<xml_diff>
--- a/04_Metricas/Metricas_G7.xlsx
+++ b/04_Metricas/Metricas_G7.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="44">
   <si>
     <t>EL TAMAÑO DEL PRODUCTO</t>
   </si>
@@ -186,63 +186,7 @@
     <t>Max</t>
   </si>
   <si>
-    <t xml:space="preserve">Establecer conexión entre microservicios.
-</t>
-  </si>
-  <si>
-    <t>Gestionar solicitudes de estudiantes.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Definir la estructura del estudiante.
-</t>
-  </si>
-  <si>
-    <t>Implementar CRUD para estudiantes.</t>
-  </si>
-  <si>
-    <t>Definir métodos para gestión de estudiantes.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Crear clases que implementen las interfaces.
-</t>
-  </si>
-  <si>
-    <t>Punto de entrada de la aplicación.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Configurar parámetros de la aplicación.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Establecer conexión con el microservicio Estudiante.
-</t>
-  </si>
-  <si>
-    <t>Configurar conexiones entre microservicios.</t>
-  </si>
-  <si>
-    <t>Gestionar solicitudes de asignaturas.</t>
-  </si>
-  <si>
-    <t>Definir la estructura de la asignatura.</t>
-  </si>
-  <si>
-    <t>Definir la relación entre asignaturas y estudiantes.</t>
-  </si>
-  <si>
-    <t>Definir la estructura del estudiante.</t>
-  </si>
-  <si>
-    <t>Implementar CRUD para asignaturas.</t>
-  </si>
-  <si>
-    <t>Definir métodos para gestión de asignaturas.</t>
-  </si>
-  <si>
-    <t>Crear clases que implementen las interfaces de asignatura.</t>
-  </si>
-  <si>
-    <t>Configurar parámetros de la aplicación.</t>
+    <t>No aplica</t>
   </si>
   <si>
     <t>Estimado</t>
@@ -277,7 +221,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -294,6 +238,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
         <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCFE2F3"/>
+        <bgColor rgb="FFCFE2F3"/>
       </patternFill>
     </fill>
   </fills>
@@ -377,7 +327,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -416,11 +366,20 @@
     <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf borderId="5" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
     <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="4" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="4" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="5" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -867,35 +826,35 @@
       </c>
     </row>
     <row r="19">
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="16">
         <f t="shared" ref="D19:F19" si="2">SUM(D10:D18)</f>
         <v>71</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E19" s="16">
         <f t="shared" si="2"/>
         <v>210</v>
       </c>
-      <c r="F19" s="10">
+      <c r="F19" s="16">
         <f t="shared" si="2"/>
         <v>2.973953824</v>
       </c>
     </row>
     <row r="20">
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="16">
         <f t="shared" ref="D20:F20" si="3">GEOMEAN(D11:D18)</f>
         <v>6.029660052</v>
       </c>
-      <c r="E20" s="10">
+      <c r="E20" s="16">
         <f t="shared" si="3"/>
         <v>18.42910769</v>
       </c>
-      <c r="F20" s="10">
+      <c r="F20" s="16">
         <f t="shared" si="3"/>
         <v>0.3271813347</v>
       </c>
@@ -969,7 +928,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="C26" s="16">
+      <c r="C26" s="17">
         <v>5.0</v>
       </c>
       <c r="D26" s="10">
@@ -984,7 +943,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="C27" s="16">
+      <c r="C27" s="17">
         <v>6.0</v>
       </c>
       <c r="D27" s="10">
@@ -999,7 +958,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="C28" s="16">
+      <c r="C28" s="17">
         <v>7.0</v>
       </c>
       <c r="D28" s="10">
@@ -1014,7 +973,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="C29" s="16">
+      <c r="C29" s="17">
         <v>8.0</v>
       </c>
       <c r="D29" s="10">
@@ -1029,7 +988,7 @@
       </c>
     </row>
     <row r="30">
-      <c r="C30" s="16">
+      <c r="C30" s="17">
         <v>9.0</v>
       </c>
       <c r="D30" s="10">
@@ -1044,7 +1003,7 @@
       </c>
     </row>
     <row r="31">
-      <c r="C31" s="16">
+      <c r="C31" s="17">
         <v>10.0</v>
       </c>
       <c r="D31" s="10">
@@ -1059,7 +1018,7 @@
       </c>
     </row>
     <row r="32">
-      <c r="C32" s="16">
+      <c r="C32" s="17">
         <v>11.0</v>
       </c>
       <c r="D32" s="10">
@@ -1074,35 +1033,35 @@
       </c>
     </row>
     <row r="33">
-      <c r="C33" s="10" t="s">
+      <c r="C33" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="D33" s="10">
+      <c r="D33" s="16">
         <f t="shared" ref="D33:F33" si="5">SUM(D24:D32)</f>
         <v>91</v>
       </c>
-      <c r="E33" s="10">
+      <c r="E33" s="16">
         <f t="shared" si="5"/>
         <v>317</v>
       </c>
-      <c r="F33" s="10">
+      <c r="F33" s="16">
         <f t="shared" si="5"/>
         <v>2.956499259</v>
       </c>
     </row>
     <row r="34">
-      <c r="C34" s="10" t="s">
+      <c r="C34" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D34" s="10">
+      <c r="D34" s="16">
         <f t="shared" ref="D34:F34" si="6">GEOMEAN(D25:D32)</f>
         <v>6.097581108</v>
       </c>
-      <c r="E34" s="10">
+      <c r="E34" s="16">
         <f t="shared" si="6"/>
         <v>21.38731439</v>
       </c>
-      <c r="F34" s="10">
+      <c r="F34" s="16">
         <f t="shared" si="6"/>
         <v>0.2851027014</v>
       </c>
@@ -1180,7 +1139,7 @@
       <c r="G4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="17">
+      <c r="H4" s="18">
         <v>45715.0</v>
       </c>
     </row>
@@ -1387,224 +1346,298 @@
       </c>
     </row>
     <row r="19">
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="16">
+        <f t="shared" ref="D19:F19" si="2">SUM(D10:D18)</f>
+        <v>71</v>
+      </c>
+      <c r="E19" s="16">
+        <f t="shared" si="2"/>
+        <v>210</v>
+      </c>
+      <c r="F19" s="16">
+        <f t="shared" si="2"/>
+        <v>2.973953824</v>
+      </c>
+      <c r="G19" s="19"/>
+    </row>
+    <row r="20">
+      <c r="C20" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="16">
+        <f t="shared" ref="D20:F20" si="3">GEOMEAN(D11:D18)</f>
+        <v>6.029660052</v>
+      </c>
+      <c r="E20" s="16">
+        <f t="shared" si="3"/>
+        <v>18.42910769</v>
+      </c>
+      <c r="F20" s="16">
+        <f t="shared" si="3"/>
+        <v>0.3271813347</v>
+      </c>
+      <c r="G20" s="9"/>
+    </row>
+    <row r="21">
+      <c r="C21" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="3"/>
-    </row>
-    <row r="20">
-      <c r="C20" s="10">
-        <v>1.0</v>
-      </c>
-      <c r="D20" s="10">
-        <v>3.0</v>
-      </c>
-      <c r="E20" s="10">
-        <v>10.0</v>
-      </c>
-      <c r="F20" s="15">
-        <f t="shared" ref="F20:F30" si="2">DIVIDE(D20,E20)</f>
-        <v>0.3</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="C21" s="10">
-        <v>2.0</v>
-      </c>
-      <c r="D21" s="10">
-        <v>5.0</v>
-      </c>
-      <c r="E21" s="10">
-        <v>21.0</v>
-      </c>
-      <c r="F21" s="15">
-        <f t="shared" si="2"/>
-        <v>0.2380952381</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>21</v>
-      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="3"/>
     </row>
     <row r="22">
       <c r="C22" s="10">
+        <v>1.0</v>
+      </c>
+      <c r="D22" s="10">
         <v>3.0</v>
       </c>
-      <c r="D22" s="10">
-        <v>30.0</v>
-      </c>
       <c r="E22" s="10">
-        <v>73.0</v>
+        <v>10.0</v>
       </c>
       <c r="F22" s="15">
-        <f t="shared" si="2"/>
-        <v>0.4109589041</v>
+        <f t="shared" ref="F22:F32" si="4">DIVIDE(D22,E22)</f>
+        <v>0.3</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23">
       <c r="C23" s="10">
+        <v>2.0</v>
+      </c>
+      <c r="D23" s="10">
+        <v>5.0</v>
+      </c>
+      <c r="E23" s="10">
+        <v>21.0</v>
+      </c>
+      <c r="F23" s="15">
+        <f t="shared" si="4"/>
+        <v>0.2380952381</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="C24" s="10">
+        <v>3.0</v>
+      </c>
+      <c r="D24" s="10">
+        <v>30.0</v>
+      </c>
+      <c r="E24" s="10">
+        <v>73.0</v>
+      </c>
+      <c r="F24" s="15">
+        <f t="shared" si="4"/>
+        <v>0.4109589041</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="C25" s="10">
         <v>4.0</v>
       </c>
-      <c r="D23" s="10">
+      <c r="D25" s="10">
         <v>13.0</v>
       </c>
-      <c r="E23" s="10">
+      <c r="E25" s="10">
         <v>62.0</v>
       </c>
-      <c r="F23" s="15">
-        <f t="shared" si="2"/>
+      <c r="F25" s="15">
+        <f t="shared" si="4"/>
         <v>0.2096774194</v>
       </c>
-      <c r="G23" s="6" t="s">
+      <c r="G25" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="24">
-      <c r="C24" s="16">
+    <row r="26">
+      <c r="C26" s="17">
         <v>5.0</v>
       </c>
-      <c r="D24" s="10">
+      <c r="D26" s="10">
         <v>7.0</v>
       </c>
-      <c r="E24" s="10">
+      <c r="E26" s="10">
         <v>28.0</v>
       </c>
-      <c r="F24" s="15">
-        <f t="shared" si="2"/>
+      <c r="F26" s="15">
+        <f t="shared" si="4"/>
         <v>0.25</v>
       </c>
-      <c r="G24" s="6" t="s">
+      <c r="G26" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="25">
-      <c r="C25" s="16">
+    <row r="27">
+      <c r="C27" s="17">
         <v>6.0</v>
       </c>
-      <c r="D25" s="10">
+      <c r="D27" s="10">
         <v>10.0</v>
       </c>
-      <c r="E25" s="10">
+      <c r="E27" s="10">
         <v>53.0</v>
       </c>
-      <c r="F25" s="15">
-        <f t="shared" si="2"/>
+      <c r="F27" s="15">
+        <f t="shared" si="4"/>
         <v>0.1886792453</v>
       </c>
-      <c r="G25" s="6" t="s">
+      <c r="G27" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26">
-      <c r="C26" s="16">
+    <row r="28">
+      <c r="C28" s="17">
         <v>7.0</v>
       </c>
-      <c r="D26" s="10">
+      <c r="D28" s="10">
         <v>2.0</v>
       </c>
-      <c r="E26" s="10">
+      <c r="E28" s="10">
         <v>5.0</v>
       </c>
-      <c r="F26" s="15">
-        <f t="shared" si="2"/>
+      <c r="F28" s="15">
+        <f t="shared" si="4"/>
         <v>0.4</v>
       </c>
-      <c r="G26" s="6" t="s">
+      <c r="G28" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="27">
-      <c r="C27" s="16">
+    <row r="29">
+      <c r="C29" s="17">
         <v>8.0</v>
       </c>
-      <c r="D27" s="10">
+      <c r="D29" s="10">
         <v>5.0</v>
       </c>
-      <c r="E27" s="10">
+      <c r="E29" s="10">
         <v>13.0</v>
       </c>
-      <c r="F27" s="15">
-        <f t="shared" si="2"/>
+      <c r="F29" s="15">
+        <f t="shared" si="4"/>
         <v>0.3846153846</v>
       </c>
-      <c r="G27" s="6" t="s">
+      <c r="G29" s="6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="28">
-      <c r="C28" s="16">
+    <row r="30">
+      <c r="C30" s="17">
         <v>9.0</v>
       </c>
-      <c r="D28" s="10">
+      <c r="D30" s="10">
         <v>15.0</v>
       </c>
-      <c r="E28" s="10">
+      <c r="E30" s="10">
         <v>61.0</v>
       </c>
-      <c r="F28" s="15">
-        <f t="shared" si="2"/>
+      <c r="F30" s="15">
+        <f t="shared" si="4"/>
         <v>0.2459016393</v>
       </c>
-      <c r="G28" s="6" t="s">
+      <c r="G30" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="29">
-      <c r="C29" s="16">
+    <row r="31">
+      <c r="C31" s="17">
         <v>10.0</v>
       </c>
-      <c r="D29" s="10">
+      <c r="D31" s="10">
         <v>2.0</v>
       </c>
-      <c r="E29" s="10">
+      <c r="E31" s="10">
         <v>12.0</v>
       </c>
-      <c r="F29" s="15">
-        <f t="shared" si="2"/>
+      <c r="F31" s="15">
+        <f t="shared" si="4"/>
         <v>0.1666666667</v>
       </c>
-      <c r="G29" s="6" t="s">
+      <c r="G31" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30">
-      <c r="C30" s="16">
+    <row r="32">
+      <c r="C32" s="17">
         <v>11.0</v>
       </c>
-      <c r="D30" s="10">
+      <c r="D32" s="10">
         <v>7.0</v>
       </c>
-      <c r="E30" s="10">
+      <c r="E32" s="10">
         <v>10.0</v>
       </c>
-      <c r="F30" s="15">
-        <f t="shared" si="2"/>
+      <c r="F32" s="15">
+        <f t="shared" si="4"/>
         <v>0.7</v>
       </c>
-      <c r="G30" s="6" t="s">
+      <c r="G32" s="6" t="s">
         <v>28</v>
       </c>
     </row>
+    <row r="33">
+      <c r="C33" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="16">
+        <f t="shared" ref="D33:F33" si="5">SUM(D24:D32)</f>
+        <v>91</v>
+      </c>
+      <c r="E33" s="16">
+        <f t="shared" si="5"/>
+        <v>317</v>
+      </c>
+      <c r="F33" s="16">
+        <f t="shared" si="5"/>
+        <v>2.956499259</v>
+      </c>
+      <c r="G33" s="19"/>
+    </row>
+    <row r="34">
+      <c r="C34" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" s="16">
+        <f t="shared" ref="D34:F34" si="6">GEOMEAN(D25:D32)</f>
+        <v>6.097581108</v>
+      </c>
+      <c r="E34" s="16">
+        <f t="shared" si="6"/>
+        <v>21.38731439</v>
+      </c>
+      <c r="F34" s="16">
+        <f t="shared" si="6"/>
+        <v>0.2851027014</v>
+      </c>
+      <c r="G34" s="9"/>
+    </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="12">
     <mergeCell ref="C10:G10"/>
     <mergeCell ref="C7:H7"/>
-    <mergeCell ref="C19:G19"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="G33:G34"/>
     <mergeCell ref="F4:F6"/>
     <mergeCell ref="E4:E6"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="G4:G5"/>
     <mergeCell ref="H4:H5"/>
     <mergeCell ref="C3:H3"/>
-    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="C21:G21"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="C7"/>
@@ -1752,13 +1785,16 @@
         <v>42</v>
       </c>
       <c r="G11" s="10">
-        <v>2.0</v>
+        <f t="shared" ref="G11:G18" si="1">MULTIPLY(H11,0.8)</f>
+        <v>4</v>
       </c>
       <c r="H11" s="10">
-        <v>5.0</v>
+        <f>'Estimación 6.3'!D11</f>
+        <v>5</v>
       </c>
       <c r="I11" s="10">
-        <v>8.0</v>
+        <f t="shared" ref="I11:I18" si="2">MULTIPLY(H11,1.2)</f>
+        <v>6</v>
       </c>
     </row>
     <row r="12">
@@ -1772,16 +1808,19 @@
         <v>22</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G12" s="10">
-        <v>20.0</v>
+        <f t="shared" si="1"/>
+        <v>24</v>
       </c>
       <c r="H12" s="10">
-        <v>30.0</v>
+        <f>'Estimación 6.3'!D12</f>
+        <v>30</v>
       </c>
       <c r="I12" s="10">
-        <v>40.0</v>
+        <f t="shared" si="2"/>
+        <v>36</v>
       </c>
     </row>
     <row r="13">
@@ -1795,16 +1834,19 @@
         <v>23</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G13" s="10">
-        <v>4.0</v>
+        <f t="shared" si="1"/>
+        <v>6.4</v>
       </c>
       <c r="H13" s="10">
-        <v>8.0</v>
+        <f>'Estimación 6.3'!D13</f>
+        <v>8</v>
       </c>
       <c r="I13" s="10">
-        <v>12.0</v>
+        <f t="shared" si="2"/>
+        <v>9.6</v>
       </c>
     </row>
     <row r="14">
@@ -1818,16 +1860,19 @@
         <v>24</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G14" s="10">
-        <v>1.0</v>
+        <f t="shared" si="1"/>
+        <v>1.6</v>
       </c>
       <c r="H14" s="10">
-        <v>2.0</v>
+        <f>'Estimación 6.3'!D14</f>
+        <v>2</v>
       </c>
       <c r="I14" s="10">
-        <v>3.0</v>
+        <f t="shared" si="2"/>
+        <v>2.4</v>
       </c>
     </row>
     <row r="15">
@@ -1841,16 +1886,19 @@
         <v>25</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G15" s="10">
-        <v>2.0</v>
+        <f t="shared" si="1"/>
+        <v>3.2</v>
       </c>
       <c r="H15" s="10">
-        <v>4.0</v>
+        <f>'Estimación 6.3'!D15</f>
+        <v>4</v>
       </c>
       <c r="I15" s="10">
-        <v>6.0</v>
+        <f t="shared" si="2"/>
+        <v>4.8</v>
       </c>
     </row>
     <row r="16">
@@ -1864,16 +1912,19 @@
         <v>26</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="G16" s="10">
-        <v>7.0</v>
+        <f t="shared" si="1"/>
+        <v>10.4</v>
       </c>
       <c r="H16" s="10">
-        <v>13.0</v>
+        <f>'Estimación 6.3'!D16</f>
+        <v>13</v>
       </c>
       <c r="I16" s="10">
-        <v>19.0</v>
+        <f t="shared" si="2"/>
+        <v>15.6</v>
       </c>
     </row>
     <row r="17">
@@ -1887,16 +1938,19 @@
         <v>27</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="G17" s="10">
-        <v>1.0</v>
+        <f t="shared" si="1"/>
+        <v>1.6</v>
       </c>
       <c r="H17" s="10">
-        <v>2.0</v>
+        <f>'Estimación 6.3'!D17</f>
+        <v>2</v>
       </c>
       <c r="I17" s="10">
-        <v>3.0</v>
+        <f t="shared" si="2"/>
+        <v>2.4</v>
       </c>
     </row>
     <row r="18">
@@ -1910,16 +1964,19 @@
         <v>28</v>
       </c>
       <c r="F18" s="10" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="G18" s="10">
-        <v>4.0</v>
+        <f t="shared" si="1"/>
+        <v>5.6</v>
       </c>
       <c r="H18" s="10">
-        <v>7.0</v>
+        <f>'Estimación 6.3'!D18</f>
+        <v>7</v>
       </c>
       <c r="I18" s="10">
-        <v>10.0</v>
+        <f t="shared" si="2"/>
+        <v>8.4</v>
       </c>
     </row>
     <row r="19">
@@ -1944,16 +2001,19 @@
         <v>29</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="G20" s="10">
-        <v>2.0</v>
+        <f t="shared" ref="G20:G30" si="3">MULTIPLY(H20,0.8)</f>
+        <v>2.4</v>
       </c>
       <c r="H20" s="10">
-        <v>3.0</v>
+        <f>'Estimación 6.3'!D22</f>
+        <v>3</v>
       </c>
       <c r="I20" s="10">
-        <v>4.0</v>
+        <f t="shared" ref="I20:I30" si="4">MULTIPLY(H20,1.2)</f>
+        <v>3.6</v>
       </c>
     </row>
     <row r="21">
@@ -1967,16 +2027,19 @@
         <v>21</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="G21" s="10">
-        <v>2.0</v>
+        <f t="shared" si="3"/>
+        <v>4</v>
       </c>
       <c r="H21" s="10">
-        <v>5.0</v>
+        <f>'Estimación 6.3'!D23</f>
+        <v>5</v>
       </c>
       <c r="I21" s="10">
-        <v>8.0</v>
+        <f t="shared" si="4"/>
+        <v>6</v>
       </c>
     </row>
     <row r="22">
@@ -1990,16 +2053,19 @@
         <v>30</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="G22" s="10">
-        <v>20.0</v>
+        <f t="shared" si="3"/>
+        <v>24</v>
       </c>
       <c r="H22" s="10">
-        <v>30.0</v>
+        <f>'Estimación 6.3'!D24</f>
+        <v>30</v>
       </c>
       <c r="I22" s="10">
-        <v>40.0</v>
+        <f t="shared" si="4"/>
+        <v>36</v>
       </c>
     </row>
     <row r="23">
@@ -2013,20 +2079,23 @@
         <v>31</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="G23" s="10">
-        <v>7.0</v>
+        <f t="shared" si="3"/>
+        <v>10.4</v>
       </c>
       <c r="H23" s="10">
-        <v>13.0</v>
+        <f>'Estimación 6.3'!D25</f>
+        <v>13</v>
       </c>
       <c r="I23" s="10">
-        <v>19.0</v>
+        <f t="shared" si="4"/>
+        <v>15.6</v>
       </c>
     </row>
     <row r="24">
-      <c r="C24" s="16">
+      <c r="C24" s="17">
         <v>5.0</v>
       </c>
       <c r="D24" s="10">
@@ -2036,20 +2105,23 @@
         <v>32</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="G24" s="10">
-        <v>7.0</v>
+        <f t="shared" si="3"/>
+        <v>5.6</v>
       </c>
       <c r="H24" s="10">
-        <v>7.0</v>
+        <f>'Estimación 6.3'!D26</f>
+        <v>7</v>
       </c>
       <c r="I24" s="10">
-        <v>19.0</v>
+        <f t="shared" si="4"/>
+        <v>8.4</v>
       </c>
     </row>
     <row r="25">
-      <c r="C25" s="16">
+      <c r="C25" s="17">
         <v>6.0</v>
       </c>
       <c r="D25" s="10">
@@ -2059,20 +2131,23 @@
         <v>33</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="G25" s="10">
-        <v>6.0</v>
+        <f t="shared" si="3"/>
+        <v>8</v>
       </c>
       <c r="H25" s="10">
-        <v>10.0</v>
+        <f>'Estimación 6.3'!D27</f>
+        <v>10</v>
       </c>
       <c r="I25" s="10">
-        <v>15.0</v>
+        <f t="shared" si="4"/>
+        <v>12</v>
       </c>
     </row>
     <row r="26">
-      <c r="C26" s="16">
+      <c r="C26" s="17">
         <v>7.0</v>
       </c>
       <c r="D26" s="10">
@@ -2082,20 +2157,23 @@
         <v>34</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="G26" s="10">
-        <v>1.0</v>
+        <f t="shared" si="3"/>
+        <v>1.6</v>
       </c>
       <c r="H26" s="10">
-        <v>2.0</v>
+        <f>'Estimación 6.3'!D28</f>
+        <v>2</v>
       </c>
       <c r="I26" s="10">
-        <v>3.0</v>
+        <f t="shared" si="4"/>
+        <v>2.4</v>
       </c>
     </row>
     <row r="27">
-      <c r="C27" s="16">
+      <c r="C27" s="17">
         <v>8.0</v>
       </c>
       <c r="D27" s="10">
@@ -2105,20 +2183,23 @@
         <v>35</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="G27" s="10">
-        <v>2.0</v>
+        <f t="shared" si="3"/>
+        <v>4</v>
       </c>
       <c r="H27" s="10">
-        <v>5.0</v>
+        <f>'Estimación 6.3'!D29</f>
+        <v>5</v>
       </c>
       <c r="I27" s="10">
-        <v>8.0</v>
+        <f t="shared" si="4"/>
+        <v>6</v>
       </c>
     </row>
     <row r="28">
-      <c r="C28" s="16">
+      <c r="C28" s="17">
         <v>9.0</v>
       </c>
       <c r="D28" s="10">
@@ -2128,20 +2209,23 @@
         <v>36</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="G28" s="10">
-        <v>10.0</v>
+        <f t="shared" si="3"/>
+        <v>12</v>
       </c>
       <c r="H28" s="10">
-        <v>15.0</v>
+        <f>'Estimación 6.3'!D30</f>
+        <v>15</v>
       </c>
       <c r="I28" s="10">
-        <v>20.0</v>
+        <f t="shared" si="4"/>
+        <v>18</v>
       </c>
     </row>
     <row r="29">
-      <c r="C29" s="16">
+      <c r="C29" s="17">
         <v>10.0</v>
       </c>
       <c r="D29" s="10">
@@ -2151,20 +2235,23 @@
         <v>27</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="G29" s="10">
-        <v>1.0</v>
+        <f t="shared" si="3"/>
+        <v>1.6</v>
       </c>
       <c r="H29" s="10">
-        <v>2.0</v>
+        <f>'Estimación 6.3'!D31</f>
+        <v>2</v>
       </c>
       <c r="I29" s="10">
-        <v>3.0</v>
+        <f t="shared" si="4"/>
+        <v>2.4</v>
       </c>
     </row>
     <row r="30">
-      <c r="C30" s="16">
+      <c r="C30" s="17">
         <v>11.0</v>
       </c>
       <c r="D30" s="10">
@@ -2174,36 +2261,39 @@
         <v>28</v>
       </c>
       <c r="F30" s="10" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="G30" s="10">
-        <v>4.0</v>
+        <f t="shared" si="3"/>
+        <v>5.6</v>
       </c>
       <c r="H30" s="10">
-        <v>7.0</v>
+        <f>'Estimación 6.3'!D32</f>
+        <v>7</v>
       </c>
       <c r="I30" s="10">
-        <v>9.0</v>
+        <f t="shared" si="4"/>
+        <v>8.4</v>
       </c>
     </row>
     <row r="31">
-      <c r="C31" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10">
-        <f t="shared" ref="G31:I31" si="1">SUM(G10:G30)</f>
-        <v>103</v>
-      </c>
-      <c r="H31" s="10">
-        <f t="shared" si="1"/>
+      <c r="C31" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16">
+        <f t="shared" ref="G31:I31" si="5">SUM(G10:G30)</f>
+        <v>136</v>
+      </c>
+      <c r="H31" s="16">
+        <f t="shared" si="5"/>
         <v>170</v>
       </c>
-      <c r="I31" s="10">
-        <f t="shared" si="1"/>
-        <v>249</v>
+      <c r="I31" s="16">
+        <f t="shared" si="5"/>
+        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>